<commit_message>
Lista de camadas atualizada
</commit_message>
<xml_diff>
--- a/notebooks/camadas.xlsx
+++ b/notebooks/camadas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -620,6 +620,20 @@
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
     </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>massa</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>geometry, cd_identificador_hidrografia_poligono, nm_acidente, cd_tipo_acidente</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>